<commit_message>
new diagram + chart of tests
</commit_message>
<xml_diff>
--- a/Miscellaneous/tests.xlsx
+++ b/Miscellaneous/tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sylve\OneDrive\Bureau\Telemetry-for-the-Formula-Student\Miscellaneous\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C532981-B50A-4553-A325-66E9C890E667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC73A321-651A-49C6-9E87-03288115F1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base system" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="38">
   <si>
     <t>Base system</t>
   </si>
@@ -135,6 +135,21 @@
   </si>
   <si>
     <t>Cache flush</t>
+  </si>
+  <si>
+    <t>canbus rate</t>
+  </si>
+  <si>
+    <t>lograte</t>
+  </si>
+  <si>
+    <t>Update on base hardware</t>
+  </si>
+  <si>
+    <t>New hardware</t>
+  </si>
+  <si>
+    <t>New hardware/nofilter</t>
   </si>
 </sst>
 </file>
@@ -470,6 +485,3136 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Base system'!$N$27:$N$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Base system'!$O$27:$O$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3400</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9725-4DA2-9DE1-E9391876FBA2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Base system'!$K$27:$K$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Base system'!$L$27:$L$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9725-4DA2-9DE1-E9391876FBA2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Base system'!$H$27:$H$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Base system'!$I$27:$I$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-9725-4DA2-9DE1-E9391876FBA2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2117103455"/>
+        <c:axId val="2117093327"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2117103455"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2117093327"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2117093327"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2117103455"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Base system'!$K$27:$K$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Base system'!$L$27:$L$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A85E-495E-912F-C217A0EA0374}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Base system'!$H$27:$H$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Base system'!$I$27:$I$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A85E-495E-912F-C217A0EA0374}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2117103455"/>
+        <c:axId val="2117093327"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2117103455"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2117093327"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2117093327"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2117103455"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Base system'!$N$27:$N$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Base system'!$O$27:$O$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3400</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D988-469D-944B-435264551DCD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Base system'!$Q$27:$Q$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Base system'!$R$27:$R$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D988-469D-944B-435264551DCD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2117103455"/>
+        <c:axId val="2117093327"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2117103455"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2117093327"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2117093327"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2117103455"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>583199</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>657494</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>133215</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02C29F1B-50E7-BB9A-3449-4970464BC37E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>567690</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>19885</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B66C0B9-0F13-4782-9E14-6A2395AE90E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>81915</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>146685</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>55110</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Graphique 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A750542-DC00-48CD-9F47-41C280EDB251}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -735,8 +3880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="AL6" sqref="AL6"/>
+    <sheetView tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,10 +3891,11 @@
     <col min="3" max="3" width="18.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" style="1" customWidth="1"/>
     <col min="5" max="9" width="14.42578125" style="1" customWidth="1"/>
-    <col min="10" max="11" width="14.42578125" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" customWidth="1"/>
+    <col min="11" max="12" width="14.42578125" style="1" customWidth="1"/>
     <col min="13" max="13" width="14.42578125" customWidth="1"/>
     <col min="14" max="14" width="13.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
     <col min="16" max="18" width="13.85546875" style="1" customWidth="1"/>
     <col min="19" max="19" width="13.42578125" style="1" customWidth="1"/>
     <col min="20" max="20" width="13.7109375" style="1" customWidth="1"/>
@@ -1692,7 +4838,24 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="H24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R24"/>
+    </row>
+    <row r="25" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R25"/>
+    </row>
     <row r="26" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>31</v>
@@ -1702,6 +4865,30 @@
       </c>
       <c r="C26" s="5" t="s">
         <v>25</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:36" x14ac:dyDescent="0.25">
@@ -1715,6 +4902,30 @@
         <f>1/B27*1000</f>
         <v>200</v>
       </c>
+      <c r="H27" s="1">
+        <v>50</v>
+      </c>
+      <c r="I27" s="1">
+        <v>1</v>
+      </c>
+      <c r="K27" s="1">
+        <v>100</v>
+      </c>
+      <c r="L27" s="1">
+        <v>1</v>
+      </c>
+      <c r="N27" s="1">
+        <v>1000</v>
+      </c>
+      <c r="O27" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>1000</v>
+      </c>
+      <c r="R27" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
@@ -1727,6 +4938,30 @@
         <f t="shared" ref="C28:C34" si="0">1/B28*1000</f>
         <v>200</v>
       </c>
+      <c r="H28" s="1">
+        <v>50</v>
+      </c>
+      <c r="I28" s="1">
+        <v>200</v>
+      </c>
+      <c r="K28" s="1">
+        <v>100</v>
+      </c>
+      <c r="L28" s="1">
+        <v>300</v>
+      </c>
+      <c r="N28" s="1">
+        <v>1000</v>
+      </c>
+      <c r="O28" s="1">
+        <v>1200</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>800</v>
+      </c>
+      <c r="R28" s="1">
+        <v>1600</v>
+      </c>
     </row>
     <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
@@ -1739,6 +4974,30 @@
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
+      <c r="H29" s="1">
+        <v>20</v>
+      </c>
+      <c r="I29" s="1">
+        <v>300</v>
+      </c>
+      <c r="K29" s="1">
+        <v>50</v>
+      </c>
+      <c r="L29" s="1">
+        <v>500</v>
+      </c>
+      <c r="N29" s="1">
+        <v>1000</v>
+      </c>
+      <c r="O29" s="1">
+        <v>2200</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>500</v>
+      </c>
+      <c r="R29" s="1">
+        <v>2500</v>
+      </c>
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
@@ -1751,6 +5010,30 @@
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
+      <c r="H30" s="1">
+        <v>10</v>
+      </c>
+      <c r="I30" s="1">
+        <v>350</v>
+      </c>
+      <c r="K30" s="1">
+        <v>20</v>
+      </c>
+      <c r="L30" s="1">
+        <v>700</v>
+      </c>
+      <c r="N30" s="1">
+        <v>1000</v>
+      </c>
+      <c r="O30" s="1">
+        <v>3400</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>200</v>
+      </c>
+      <c r="R30" s="1">
+        <v>2500</v>
+      </c>
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
@@ -1763,6 +5046,30 @@
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
+      <c r="H31" s="1">
+        <v>5</v>
+      </c>
+      <c r="I31" s="1">
+        <v>400</v>
+      </c>
+      <c r="K31" s="1">
+        <v>10</v>
+      </c>
+      <c r="L31" s="1">
+        <v>800</v>
+      </c>
+      <c r="N31" s="1">
+        <v>1</v>
+      </c>
+      <c r="O31" s="1">
+        <v>3400</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>1</v>
+      </c>
+      <c r="R31" s="1">
+        <v>3000</v>
+      </c>
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
@@ -1775,8 +5082,26 @@
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
+      <c r="H32" s="1">
+        <v>1</v>
+      </c>
+      <c r="I32" s="1">
+        <v>400</v>
+      </c>
+      <c r="K32" s="1">
+        <v>1</v>
+      </c>
+      <c r="L32" s="1">
+        <v>800</v>
+      </c>
+      <c r="N32" s="1">
+        <v>200</v>
+      </c>
+      <c r="O32" s="1">
+        <v>3400</v>
+      </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>27</v>
       </c>
@@ -1787,8 +5112,14 @@
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
+      <c r="N33" s="1">
+        <v>500</v>
+      </c>
+      <c r="O33" s="1">
+        <v>3400</v>
+      </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16" t="s">
         <v>28</v>
       </c>
@@ -1799,12 +5130,18 @@
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
+      <c r="N34" s="1">
+        <v>1000</v>
+      </c>
+      <c r="O34" s="1">
+        <v>3400</v>
+      </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
       <c r="C35" s="7"/>
     </row>
-    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>29</v>
       </c>
@@ -1813,12 +5150,13 @@
         <f>SUM(C27:C34)</f>
         <v>1600</v>
       </c>
+      <c r="O36" s="1"/>
     </row>
-    <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6"/>
       <c r="C37" s="7"/>
     </row>
-    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="19" t="s">
         <v>30</v>
       </c>
@@ -1830,8 +5168,10 @@
         <f>1000/B38</f>
         <v>1000</v>
       </c>
+      <c r="O38" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>